<commit_message>
yeni test sayfasi bilgileri, ApachePOI - Cucumber 1, Master Report projeden cikarildi, ExcelReport 1
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber_Kursu3\src\test\java\ApachePOI\resource\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="396" windowWidth="17280" windowHeight="8976" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="testCitizen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -63,59 +58,59 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulkemis11</t>
-  </si>
-  <si>
-    <t>ulkemis22</t>
-  </si>
-  <si>
-    <t>ulkemis33</t>
-  </si>
-  <si>
-    <t>ulkemis44</t>
-  </si>
-  <si>
-    <t>ulkemis55</t>
-  </si>
-  <si>
-    <t>ulkemis66</t>
-  </si>
-  <si>
-    <t>ulkemis77</t>
-  </si>
-  <si>
-    <t>ulkemis88</t>
-  </si>
-  <si>
-    <t>uis11</t>
-  </si>
-  <si>
-    <t>uis21</t>
-  </si>
-  <si>
-    <t>uis31</t>
-  </si>
-  <si>
-    <t>uis41</t>
-  </si>
-  <si>
-    <t>uis51</t>
-  </si>
-  <si>
-    <t>uis61</t>
-  </si>
-  <si>
-    <t>uis71</t>
-  </si>
-  <si>
-    <t>uis81</t>
+    <t>uisve111</t>
+  </si>
+  <si>
+    <t>uisve112</t>
+  </si>
+  <si>
+    <t>uisve113</t>
+  </si>
+  <si>
+    <t>uisve114</t>
+  </si>
+  <si>
+    <t>uisve115</t>
+  </si>
+  <si>
+    <t>uisve116</t>
+  </si>
+  <si>
+    <t>uisve117</t>
+  </si>
+  <si>
+    <t>uisve118</t>
+  </si>
+  <si>
+    <t>ulkemiz111</t>
+  </si>
+  <si>
+    <t>ulkemiz112</t>
+  </si>
+  <si>
+    <t>ulkemiz113</t>
+  </si>
+  <si>
+    <t>ulkemiz114</t>
+  </si>
+  <si>
+    <t>ulkemiz115</t>
+  </si>
+  <si>
+    <t>ulkemiz116</t>
+  </si>
+  <si>
+    <t>ulkemiz117</t>
+  </si>
+  <si>
+    <t>ulkemiz118</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,7 +144,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -207,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -242,7 +237,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -419,23 +414,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -465,7 +460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -473,7 +468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -481,7 +476,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,7 +484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -497,7 +492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -509,25 +504,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -541,13 +536,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -561,13 +556,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -581,13 +576,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -601,13 +596,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -621,13 +616,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -641,13 +636,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -661,12 +656,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>

</xml_diff>